<commit_message>
var control us + stationnarite var controle
</commit_message>
<xml_diff>
--- a/code/data.xlsx
+++ b/code/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\Desktop\Github\GitHub\StatApp\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D071FBE-2C7F-4FC9-9BB8-43BBF81F6FC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51125773-441A-495C-9645-7089F1AB0D39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{300B3C8C-D0C8-4F5C-B1F9-63352E12FFD4}"/>
   </bookViews>
@@ -1545,7 +1545,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="15">
   <si>
     <t>chomage</t>
   </si>
@@ -1581,9 +1581,6 @@
   </si>
   <si>
     <t>cpi</t>
-  </si>
-  <si>
-    <t>taux_st</t>
   </si>
   <si>
     <t>dwelling stocks</t>
@@ -2027,7 +2024,7 @@
   <dimension ref="A1:M194"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2047,7 +2044,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>9</v>
@@ -7012,10 +7009,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8193407F-CECE-4DA6-A9C8-D7EDBCD1DB3A}">
-  <dimension ref="A1:N108"/>
+  <dimension ref="A1:O108"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2:K106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7030,14 +7027,15 @@
     <col min="8" max="8" width="8.36328125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="6.54296875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="6.90625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4.90625" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.90625" customWidth="1"/>
+    <col min="12" max="12" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.90625" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="13.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>9</v>
@@ -7052,10 +7050,10 @@
         <v>10</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H1" s="8" t="s">
         <v>0</v>
@@ -7064,19 +7062,22 @@
         <v>2</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="K1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="M1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="N1" s="8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="9">
         <v>35765</v>
       </c>
@@ -7107,18 +7108,22 @@
       <c r="J2" s="8">
         <v>5.73</v>
       </c>
-      <c r="K2" s="7">
+      <c r="K2" s="8">
+        <f>I2-J2</f>
+        <v>0.17666666666666941</v>
+      </c>
+      <c r="L2" s="7">
         <v>101.3878</v>
       </c>
-      <c r="L2" s="8">
+      <c r="M2" s="8">
         <v>0.68349530000000003</v>
       </c>
-      <c r="M2" s="11">
+      <c r="N2" s="11">
         <v>5583844</v>
       </c>
-      <c r="N2" s="10"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O2" s="10"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" s="9">
         <v>35855</v>
       </c>
@@ -7149,18 +7154,22 @@
       <c r="J3" s="8">
         <v>5.5533333333333301</v>
       </c>
-      <c r="K3" s="7">
+      <c r="K3" s="8">
+        <f t="shared" ref="K3:K66" si="0">I3-J3</f>
+        <v>3.3333333333339432E-2</v>
+      </c>
+      <c r="L3" s="7">
         <v>101.5625</v>
       </c>
-      <c r="L3" s="8">
+      <c r="M3" s="8">
         <v>0.68574550000000001</v>
       </c>
-      <c r="M3" s="11">
+      <c r="N3" s="11">
         <v>5698139</v>
       </c>
-      <c r="N3" s="10"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O3" s="10"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" s="9">
         <v>35947</v>
       </c>
@@ -7191,18 +7200,22 @@
       <c r="J4" s="8">
         <v>5.59</v>
       </c>
-      <c r="K4" s="7">
+      <c r="K4" s="8">
+        <f t="shared" si="0"/>
+        <v>6.6666666666703733E-3</v>
+      </c>
+      <c r="L4" s="7">
         <v>101.47020000000001</v>
       </c>
-      <c r="L4" s="8">
+      <c r="M4" s="8">
         <v>0.68926136666666682</v>
       </c>
-      <c r="M4" s="11">
+      <c r="N4" s="11">
         <v>5858251</v>
       </c>
-      <c r="N4" s="10"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O4" s="10"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" s="9">
         <v>36039</v>
       </c>
@@ -7233,18 +7246,22 @@
       <c r="J5" s="8">
         <v>5.5266666666666699</v>
       </c>
-      <c r="K5" s="7">
+      <c r="K5" s="8">
+        <f t="shared" si="0"/>
+        <v>-0.32333333333334036</v>
+      </c>
+      <c r="L5" s="7">
         <v>101.2901</v>
       </c>
-      <c r="L5" s="8">
+      <c r="M5" s="8">
         <v>0.69249603333333343</v>
       </c>
-      <c r="M5" s="11">
+      <c r="N5" s="11">
         <v>6013008</v>
       </c>
-      <c r="N5" s="10"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O5" s="10"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" s="9">
         <v>36130</v>
       </c>
@@ -7275,18 +7292,22 @@
       <c r="J6" s="8">
         <v>5.1966666666666699</v>
       </c>
-      <c r="K6" s="7">
+      <c r="K6" s="8">
+        <f t="shared" si="0"/>
+        <v>-0.52666666666666995</v>
+      </c>
+      <c r="L6" s="7">
         <v>101.51949999999999</v>
       </c>
-      <c r="L6" s="8">
+      <c r="M6" s="8">
         <v>0.69502753333333334</v>
       </c>
-      <c r="M6" s="11">
+      <c r="N6" s="11">
         <v>6144124</v>
       </c>
-      <c r="N6" s="10"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O6" s="10"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" s="9">
         <v>36220</v>
       </c>
@@ -7317,18 +7338,22 @@
       <c r="J7" s="8">
         <v>4.9000000000000004</v>
       </c>
-      <c r="K7" s="7">
+      <c r="K7" s="8">
+        <f t="shared" si="0"/>
+        <v>8.3333333333329485E-2</v>
+      </c>
+      <c r="L7" s="7">
         <v>101.7591</v>
       </c>
-      <c r="L7" s="8">
+      <c r="M7" s="8">
         <v>0.70023106666666646</v>
       </c>
-      <c r="M7" s="11">
+      <c r="N7" s="11">
         <v>6261603</v>
       </c>
-      <c r="N7" s="10"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O7" s="10"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" s="9">
         <v>36312</v>
       </c>
@@ -7359,18 +7384,22 @@
       <c r="J8" s="8">
         <v>4.9766666666666701</v>
       </c>
-      <c r="K8" s="7">
+      <c r="K8" s="8">
+        <f t="shared" si="0"/>
+        <v>0.56333333333332991</v>
+      </c>
+      <c r="L8" s="7">
         <v>101.7911</v>
       </c>
-      <c r="L8" s="8">
+      <c r="M8" s="8">
         <v>0.70543459999999991</v>
       </c>
-      <c r="M8" s="11">
+      <c r="N8" s="11">
         <v>6439691</v>
       </c>
-      <c r="N8" s="10"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O8" s="10"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" s="9">
         <v>36404</v>
       </c>
@@ -7401,18 +7430,22 @@
       <c r="J9" s="8">
         <v>5.3833333333333302</v>
       </c>
-      <c r="K9" s="7">
+      <c r="K9" s="8">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="L9" s="7">
         <v>101.93810000000001</v>
       </c>
-      <c r="L9" s="8">
+      <c r="M9" s="8">
         <v>0.71063820000000011</v>
       </c>
-      <c r="M9" s="11">
+      <c r="N9" s="11">
         <v>6611804</v>
       </c>
-      <c r="N9" s="10"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O9" s="10"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" s="9">
         <v>36495</v>
       </c>
@@ -7443,18 +7476,22 @@
       <c r="J10" s="8">
         <v>6.06</v>
       </c>
-      <c r="K10" s="7">
+      <c r="K10" s="8">
+        <f t="shared" si="0"/>
+        <v>8.0000000000000071E-2</v>
+      </c>
+      <c r="L10" s="7">
         <v>102.2227</v>
       </c>
-      <c r="L10" s="8">
+      <c r="M10" s="8">
         <v>0.71767003333333335</v>
       </c>
-      <c r="M10" s="11">
+      <c r="N10" s="11">
         <v>6771632</v>
       </c>
-      <c r="N10" s="10"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O10" s="10"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" s="9">
         <v>36586</v>
       </c>
@@ -7485,18 +7522,22 @@
       <c r="J11" s="8">
         <v>6.0333333333333297</v>
       </c>
-      <c r="K11" s="7">
+      <c r="K11" s="8">
+        <f t="shared" si="0"/>
+        <v>0.44666666666667076</v>
+      </c>
+      <c r="L11" s="7">
         <v>102.29559999999999</v>
       </c>
-      <c r="L11" s="8">
+      <c r="M11" s="8">
         <v>0.72329549999999998</v>
       </c>
-      <c r="M11" s="11">
+      <c r="N11" s="11">
         <v>7104272</v>
       </c>
-      <c r="N11" s="10"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O11" s="10"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" s="9">
         <v>36678</v>
       </c>
@@ -7527,18 +7568,22 @@
       <c r="J12" s="8">
         <v>6.5733333333333297</v>
       </c>
-      <c r="K12" s="7">
+      <c r="K12" s="8">
+        <f t="shared" si="0"/>
+        <v>-0.3966666666666594</v>
+      </c>
+      <c r="L12" s="7">
         <v>102.2345</v>
       </c>
-      <c r="L12" s="8">
+      <c r="M12" s="8">
         <v>0.72990549999999998</v>
       </c>
-      <c r="M12" s="11">
+      <c r="N12" s="11">
         <v>7441365</v>
       </c>
-      <c r="N12" s="10"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O12" s="10"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13" s="9">
         <v>36770</v>
       </c>
@@ -7569,18 +7614,22 @@
       <c r="J13" s="8">
         <v>6.6266666666666696</v>
       </c>
-      <c r="K13" s="7">
+      <c r="K13" s="8">
+        <f t="shared" si="0"/>
+        <v>-0.73333333333333961</v>
+      </c>
+      <c r="L13" s="7">
         <v>102.0427</v>
       </c>
-      <c r="L13" s="8">
+      <c r="M13" s="8">
         <v>0.73510900000000001</v>
       </c>
-      <c r="M13" s="11">
+      <c r="N13" s="11">
         <v>7730777</v>
       </c>
-      <c r="N13" s="10"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O13" s="10"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14" s="9">
         <v>36861</v>
       </c>
@@ -7611,18 +7660,22 @@
       <c r="J14" s="8">
         <v>6.59</v>
       </c>
-      <c r="K14" s="7">
+      <c r="K14" s="8">
+        <f t="shared" si="0"/>
+        <v>-1.0233333333333299</v>
+      </c>
+      <c r="L14" s="7">
         <v>101.60850000000001</v>
       </c>
-      <c r="L14" s="8">
+      <c r="M14" s="8">
         <v>0.74214086666666679</v>
       </c>
-      <c r="M14" s="11">
+      <c r="N14" s="11">
         <v>8028747</v>
       </c>
-      <c r="N14" s="10"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O14" s="10"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15" s="9">
         <v>36951</v>
       </c>
@@ -7653,18 +7706,22 @@
       <c r="J15" s="8">
         <v>5.2566666666666704</v>
       </c>
-      <c r="K15" s="7">
+      <c r="K15" s="8">
+        <f t="shared" si="0"/>
+        <v>-0.20666666666667055</v>
+      </c>
+      <c r="L15" s="7">
         <v>101.1349</v>
       </c>
-      <c r="L15" s="8">
+      <c r="M15" s="8">
         <v>0.74734443333333345</v>
       </c>
-      <c r="M15" s="11">
+      <c r="N15" s="11">
         <v>8647985</v>
       </c>
-      <c r="N15" s="10"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O15" s="10"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16" s="9">
         <v>37043</v>
       </c>
@@ -7695,18 +7752,22 @@
       <c r="J16" s="8">
         <v>4.0966666666666702</v>
       </c>
-      <c r="K16" s="7">
+      <c r="K16" s="8">
+        <f t="shared" si="0"/>
+        <v>1.1733333333333293</v>
+      </c>
+      <c r="L16" s="7">
         <v>100.98390000000001</v>
       </c>
-      <c r="L16" s="8">
+      <c r="M16" s="8">
         <v>0.74945396666666664</v>
       </c>
-      <c r="M16" s="11">
+      <c r="N16" s="11">
         <v>8875217</v>
       </c>
-      <c r="N16" s="10"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O16" s="10"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A17" s="9">
         <v>37135</v>
       </c>
@@ -7737,18 +7798,22 @@
       <c r="J17" s="8">
         <v>3.33666666666667</v>
       </c>
-      <c r="K17" s="7">
+      <c r="K17" s="8">
+        <f t="shared" si="0"/>
+        <v>1.6433333333333304</v>
+      </c>
+      <c r="L17" s="7">
         <v>100.4405</v>
       </c>
-      <c r="L17" s="8">
+      <c r="M17" s="8">
         <v>0.74889143333333319</v>
       </c>
-      <c r="M17" s="11">
+      <c r="N17" s="11">
         <v>9105610</v>
       </c>
-      <c r="N17" s="10"/>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O17" s="10"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A18" s="9">
         <v>37226</v>
       </c>
@@ -7779,18 +7844,22 @@
       <c r="J18" s="8">
         <v>2.0566666666666702</v>
       </c>
-      <c r="K18" s="7">
+      <c r="K18" s="8">
+        <f t="shared" si="0"/>
+        <v>2.7133333333333294</v>
+      </c>
+      <c r="L18" s="7">
         <v>100.55880000000001</v>
       </c>
-      <c r="L18" s="8">
+      <c r="M18" s="8">
         <v>0.75128226666666675</v>
       </c>
-      <c r="M18" s="11">
+      <c r="N18" s="11">
         <v>9338527</v>
       </c>
-      <c r="N18" s="10"/>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O18" s="10"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A19" s="9">
         <v>37316</v>
       </c>
@@ -7821,18 +7890,22 @@
       <c r="J19" s="8">
         <v>1.8233333333333299</v>
       </c>
-      <c r="K19" s="7">
+      <c r="K19" s="8">
+        <f t="shared" si="0"/>
+        <v>3.2533333333333401</v>
+      </c>
+      <c r="L19" s="7">
         <v>100.95829999999999</v>
       </c>
-      <c r="L19" s="8">
+      <c r="M19" s="8">
         <v>0.75718896666666669</v>
       </c>
-      <c r="M19" s="11">
+      <c r="N19" s="11">
         <v>9578867</v>
       </c>
-      <c r="N19" s="10"/>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O19" s="10"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A20" s="9">
         <v>37408</v>
       </c>
@@ -7863,18 +7936,22 @@
       <c r="J20" s="8">
         <v>1.8333333333333299</v>
       </c>
-      <c r="K20" s="7">
+      <c r="K20" s="8">
+        <f t="shared" si="0"/>
+        <v>3.2666666666666697</v>
+      </c>
+      <c r="L20" s="7">
         <v>100.8595</v>
       </c>
-      <c r="L20" s="8">
+      <c r="M20" s="8">
         <v>0.76126749999999999</v>
       </c>
-      <c r="M20" s="11">
+      <c r="N20" s="11">
         <v>9757440</v>
       </c>
-      <c r="N20" s="10"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O20" s="10"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A21" s="9">
         <v>37500</v>
       </c>
@@ -7905,18 +7982,22 @@
       <c r="J21" s="8">
         <v>1.76</v>
       </c>
-      <c r="K21" s="7">
+      <c r="K21" s="8">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="L21" s="7">
         <v>100.41240000000001</v>
       </c>
-      <c r="L21" s="8">
+      <c r="M21" s="8">
         <v>0.7657678333333332</v>
       </c>
-      <c r="M21" s="11">
+      <c r="N21" s="11">
         <v>9929696</v>
       </c>
-      <c r="N21" s="10"/>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O21" s="10"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A22" s="9">
         <v>37591</v>
       </c>
@@ -7947,18 +8028,22 @@
       <c r="J22" s="8">
         <v>1.4866666666666699</v>
       </c>
-      <c r="K22" s="7">
+      <c r="K22" s="8">
+        <f t="shared" si="0"/>
+        <v>2.5200000000000005</v>
+      </c>
+      <c r="L22" s="7">
         <v>99.995670000000004</v>
       </c>
-      <c r="L22" s="8">
+      <c r="M22" s="8">
         <v>0.77364353333333324</v>
       </c>
-      <c r="M22" s="11">
+      <c r="N22" s="11">
         <v>10099331</v>
       </c>
-      <c r="N22" s="10"/>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O22" s="10"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A23" s="9">
         <v>37681</v>
       </c>
@@ -7989,18 +8074,22 @@
       <c r="J23" s="8">
         <v>1.2633333333333301</v>
       </c>
-      <c r="K23" s="7">
+      <c r="K23" s="8">
+        <f t="shared" si="0"/>
+        <v>2.6566666666666698</v>
+      </c>
+      <c r="L23" s="7">
         <v>99.612139999999997</v>
       </c>
-      <c r="L23" s="8">
+      <c r="M23" s="8">
         <v>0.77237783333333321</v>
       </c>
-      <c r="M23" s="11">
+      <c r="N23" s="11">
         <v>10300888</v>
       </c>
-      <c r="N23" s="10"/>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O23" s="10"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A24" s="9">
         <v>37773</v>
       </c>
@@ -8031,18 +8120,22 @@
       <c r="J24" s="8">
         <v>1.1666666666666701</v>
       </c>
-      <c r="K24" s="7">
+      <c r="K24" s="8">
+        <f t="shared" si="0"/>
+        <v>2.45333333333333</v>
+      </c>
+      <c r="L24" s="7">
         <v>100.2953</v>
       </c>
-      <c r="L24" s="8">
+      <c r="M24" s="8">
         <v>0.77814386666666679</v>
       </c>
-      <c r="M24" s="11">
+      <c r="N24" s="11">
         <v>10444648</v>
       </c>
-      <c r="N24" s="10"/>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O24" s="10"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A25" s="9">
         <v>37865</v>
       </c>
@@ -8073,18 +8166,22 @@
       <c r="J25" s="8">
         <v>1.07</v>
       </c>
-      <c r="K25" s="7">
+      <c r="K25" s="8">
+        <f t="shared" si="0"/>
+        <v>3.1633333333333296</v>
+      </c>
+      <c r="L25" s="7">
         <v>100.36499999999999</v>
       </c>
-      <c r="L25" s="8">
+      <c r="M25" s="8">
         <v>0.78109726666666657</v>
       </c>
-      <c r="M25" s="11">
+      <c r="N25" s="11">
         <v>10617047</v>
       </c>
-      <c r="N25" s="10"/>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O25" s="10"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A26" s="9">
         <v>37956</v>
       </c>
@@ -8115,18 +8212,22 @@
       <c r="J26" s="8">
         <v>1.1033333333333299</v>
       </c>
-      <c r="K26" s="7">
+      <c r="K26" s="8">
+        <f t="shared" si="0"/>
+        <v>3.1833333333333398</v>
+      </c>
+      <c r="L26" s="7">
         <v>100.7068</v>
       </c>
-      <c r="L26" s="8">
+      <c r="M26" s="8">
         <v>0.78770719999999994</v>
       </c>
-      <c r="M26" s="11">
+      <c r="N26" s="11">
         <v>10840672</v>
       </c>
-      <c r="N26" s="10"/>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O26" s="10"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A27" s="9">
         <v>38047</v>
       </c>
@@ -8157,18 +8258,22 @@
       <c r="J27" s="8">
         <v>1.0533333333333299</v>
       </c>
-      <c r="K27" s="7">
+      <c r="K27" s="8">
+        <f t="shared" si="0"/>
+        <v>2.9666666666666694</v>
+      </c>
+      <c r="L27" s="7">
         <v>100.7903</v>
       </c>
-      <c r="L27" s="8">
+      <c r="M27" s="8">
         <v>0.79389523333333345</v>
       </c>
-      <c r="M27" s="11">
+      <c r="N27" s="11">
         <v>11356175</v>
       </c>
-      <c r="N27" s="10"/>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O27" s="10"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A28" s="9">
         <v>38139</v>
       </c>
@@ -8199,18 +8304,22 @@
       <c r="J28" s="8">
         <v>1.2466666666666699</v>
       </c>
-      <c r="K28" s="7">
+      <c r="K28" s="8">
+        <f t="shared" si="0"/>
+        <v>3.3533333333333299</v>
+      </c>
+      <c r="L28" s="7">
         <v>100.7705</v>
       </c>
-      <c r="L28" s="8">
+      <c r="M28" s="8">
         <v>0.79895816666666675</v>
       </c>
-      <c r="M28" s="11">
+      <c r="N28" s="11">
         <v>11699256</v>
       </c>
-      <c r="N28" s="10"/>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O28" s="10"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A29" s="9">
         <v>38231</v>
       </c>
@@ -8241,18 +8350,22 @@
       <c r="J29" s="8">
         <v>1.70333333333333</v>
       </c>
-      <c r="K29" s="7">
+      <c r="K29" s="8">
+        <f t="shared" si="0"/>
+        <v>2.6</v>
+      </c>
+      <c r="L29" s="7">
         <v>100.8052</v>
       </c>
-      <c r="L29" s="8">
+      <c r="M29" s="8">
         <v>0.80753699999999995</v>
       </c>
-      <c r="M29" s="11">
+      <c r="N29" s="11">
         <v>12181836</v>
       </c>
-      <c r="N29" s="10"/>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O29" s="10"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A30" s="9">
         <v>38322</v>
       </c>
@@ -8283,18 +8396,22 @@
       <c r="J30" s="8">
         <v>2.25</v>
       </c>
-      <c r="K30" s="7">
+      <c r="K30" s="8">
+        <f t="shared" si="0"/>
+        <v>1.9233333333333302</v>
+      </c>
+      <c r="L30" s="7">
         <v>100.9564</v>
       </c>
-      <c r="L30" s="8">
+      <c r="M30" s="8">
         <v>0.81161546666666651</v>
       </c>
-      <c r="M30" s="11">
+      <c r="N30" s="11">
         <v>12622776</v>
       </c>
-      <c r="N30" s="10"/>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O30" s="10"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A31" s="9">
         <v>38412</v>
       </c>
@@ -8325,18 +8442,22 @@
       <c r="J31" s="8">
         <v>2.7833333333333301</v>
       </c>
-      <c r="K31" s="7">
+      <c r="K31" s="8">
+        <f t="shared" si="0"/>
+        <v>1.5133333333333403</v>
+      </c>
+      <c r="L31" s="7">
         <v>100.8764</v>
       </c>
-      <c r="L31" s="8">
+      <c r="M31" s="8">
         <v>0.81710036666666663</v>
       </c>
-      <c r="M31" s="11">
+      <c r="N31" s="11">
         <v>13060948</v>
       </c>
-      <c r="N31" s="10"/>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O31" s="10"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A32" s="9">
         <v>38504</v>
       </c>
@@ -8367,18 +8488,22 @@
       <c r="J32" s="8">
         <v>3.23</v>
       </c>
-      <c r="K32" s="7">
+      <c r="K32" s="8">
+        <f t="shared" si="0"/>
+        <v>0.93000000000000016</v>
+      </c>
+      <c r="L32" s="7">
         <v>100.7131</v>
       </c>
-      <c r="L32" s="8">
+      <c r="M32" s="8">
         <v>0.82947633333333348</v>
       </c>
-      <c r="M32" s="11">
+      <c r="N32" s="11">
         <v>13470538</v>
       </c>
-      <c r="N32" s="10"/>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O32" s="10"/>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A33" s="9">
         <v>38596</v>
       </c>
@@ -8409,18 +8534,22 @@
       <c r="J33" s="8">
         <v>3.7366666666666699</v>
       </c>
-      <c r="K33" s="7">
+      <c r="K33" s="8">
+        <f t="shared" si="0"/>
+        <v>0.47666666666666035</v>
+      </c>
+      <c r="L33" s="7">
         <v>100.2261</v>
       </c>
-      <c r="L33" s="8">
+      <c r="M33" s="8">
         <v>0.83721143333333325</v>
       </c>
-      <c r="M33" s="11">
+      <c r="N33" s="11">
         <v>13950816</v>
       </c>
-      <c r="N33" s="10"/>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O33" s="10"/>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A34" s="9">
         <v>38687</v>
       </c>
@@ -8451,18 +8580,22 @@
       <c r="J34" s="8">
         <v>4.2966666666666704</v>
       </c>
-      <c r="K34" s="7">
+      <c r="K34" s="8">
+        <f t="shared" si="0"/>
+        <v>0.1933333333333298</v>
+      </c>
+      <c r="L34" s="7">
         <v>100.7509</v>
       </c>
-      <c r="L34" s="8">
+      <c r="M34" s="8">
         <v>0.84157113333333344</v>
       </c>
-      <c r="M34" s="11">
+      <c r="N34" s="11">
         <v>14368275</v>
       </c>
-      <c r="N34" s="10"/>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O34" s="10"/>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A35" s="9">
         <v>38777</v>
       </c>
@@ -8493,18 +8626,22 @@
       <c r="J35" s="8">
         <v>4.72</v>
       </c>
-      <c r="K35" s="7">
+      <c r="K35" s="8">
+        <f t="shared" si="0"/>
+        <v>-0.14999999999999947</v>
+      </c>
+      <c r="L35" s="7">
         <v>100.9787</v>
       </c>
-      <c r="L35" s="8">
+      <c r="M35" s="8">
         <v>0.84916553333333322</v>
       </c>
-      <c r="M35" s="11">
+      <c r="N35" s="11">
         <v>14152581</v>
       </c>
-      <c r="N35" s="10"/>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O35" s="10"/>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A36" s="9">
         <v>38869</v>
       </c>
@@ -8535,18 +8672,22 @@
       <c r="J36" s="8">
         <v>5.1766666666666703</v>
       </c>
-      <c r="K36" s="7">
+      <c r="K36" s="8">
+        <f t="shared" si="0"/>
+        <v>-0.10666666666667002</v>
+      </c>
+      <c r="L36" s="7">
         <v>100.6105</v>
       </c>
-      <c r="L36" s="8">
+      <c r="M36" s="8">
         <v>0.85718179999999999</v>
       </c>
-      <c r="M36" s="11">
+      <c r="N36" s="11">
         <v>14226415</v>
       </c>
-      <c r="N36" s="10"/>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O36" s="10"/>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A37" s="9">
         <v>38961</v>
       </c>
@@ -8577,18 +8718,22 @@
       <c r="J37" s="8">
         <v>5.39333333333333</v>
       </c>
-      <c r="K37" s="7">
+      <c r="K37" s="8">
+        <f t="shared" si="0"/>
+        <v>-0.49666666666665993</v>
+      </c>
+      <c r="L37" s="7">
         <v>100.75660000000001</v>
       </c>
-      <c r="L37" s="8">
+      <c r="M37" s="8">
         <v>0.85366589999999998</v>
       </c>
-      <c r="M37" s="11">
+      <c r="N37" s="11">
         <v>14260853</v>
       </c>
-      <c r="N37" s="10"/>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O37" s="10"/>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A38" s="9">
         <v>39052</v>
       </c>
@@ -8619,18 +8764,22 @@
       <c r="J38" s="8">
         <v>5.3233333333333297</v>
       </c>
-      <c r="K38" s="7">
+      <c r="K38" s="8">
+        <f t="shared" si="0"/>
+        <v>-0.6933333333333298</v>
+      </c>
+      <c r="L38" s="7">
         <v>101.1283</v>
       </c>
-      <c r="L38" s="8">
+      <c r="M38" s="8">
         <v>0.86203523333333321</v>
       </c>
-      <c r="M38" s="11">
+      <c r="N38" s="11">
         <v>14189922</v>
       </c>
-      <c r="N38" s="10"/>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O38" s="10"/>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A39" s="9">
         <v>39142</v>
       </c>
@@ -8661,18 +8810,22 @@
       <c r="J39" s="8">
         <v>5.31</v>
       </c>
-      <c r="K39" s="7">
+      <c r="K39" s="8">
+        <f t="shared" si="0"/>
+        <v>-0.62999999999999989</v>
+      </c>
+      <c r="L39" s="7">
         <v>100.9933</v>
       </c>
-      <c r="L39" s="8">
+      <c r="M39" s="8">
         <v>0.87179820000000008</v>
       </c>
-      <c r="M39" s="11">
+      <c r="N39" s="11">
         <v>13741739</v>
       </c>
-      <c r="N39" s="10"/>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O39" s="10"/>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A40" s="9">
         <v>39234</v>
       </c>
@@ -8703,18 +8856,22 @@
       <c r="J40" s="8">
         <v>5.31666666666667</v>
       </c>
-      <c r="K40" s="7">
+      <c r="K40" s="8">
+        <f t="shared" si="0"/>
+        <v>-0.46999999999999975</v>
+      </c>
+      <c r="L40" s="7">
         <v>100.9618</v>
       </c>
-      <c r="L40" s="8">
+      <c r="M40" s="8">
         <v>0.87731680000000001</v>
       </c>
-      <c r="M40" s="11">
+      <c r="N40" s="11">
         <v>13438697</v>
       </c>
-      <c r="N40" s="10"/>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O40" s="10"/>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A41" s="9">
         <v>39326</v>
       </c>
@@ -8745,18 +8902,22 @@
       <c r="J41" s="8">
         <v>5.4233333333333302</v>
       </c>
-      <c r="K41" s="7">
+      <c r="K41" s="8">
+        <f t="shared" si="0"/>
+        <v>-0.6933333333333298</v>
+      </c>
+      <c r="L41" s="7">
         <v>100.57</v>
       </c>
-      <c r="L41" s="8">
+      <c r="M41" s="8">
         <v>0.8880783333333333</v>
       </c>
-      <c r="M41" s="11">
+      <c r="N41" s="11">
         <v>13075258</v>
       </c>
-      <c r="N41" s="10"/>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O41" s="10"/>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A42" s="9">
         <v>39417</v>
       </c>
@@ -8787,18 +8948,22 @@
       <c r="J42" s="8">
         <v>5.0233333333333299</v>
       </c>
-      <c r="K42" s="7">
+      <c r="K42" s="8">
+        <f t="shared" si="0"/>
+        <v>-0.76333333333333009</v>
+      </c>
+      <c r="L42" s="7">
         <v>99.846689999999995</v>
       </c>
-      <c r="L42" s="8">
+      <c r="M42" s="8">
         <v>0.89769790000000005</v>
       </c>
-      <c r="M42" s="11">
+      <c r="N42" s="11">
         <v>12638719</v>
       </c>
-      <c r="N42" s="10"/>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O42" s="10"/>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A43" s="9">
         <v>39508</v>
       </c>
@@ -8829,18 +8994,22 @@
       <c r="J43" s="8">
         <v>3.23</v>
       </c>
-      <c r="K43" s="7">
+      <c r="K43" s="8">
+        <f t="shared" si="0"/>
+        <v>0.43333333333333002</v>
+      </c>
+      <c r="L43" s="7">
         <v>98.942830000000001</v>
       </c>
-      <c r="L43" s="8">
+      <c r="M43" s="8">
         <v>0.90937639999999997</v>
       </c>
-      <c r="M43" s="11">
+      <c r="N43" s="11">
         <v>11881884</v>
       </c>
-      <c r="N43" s="10"/>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O43" s="10"/>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A44" s="9">
         <v>39600</v>
       </c>
@@ -8871,18 +9040,22 @@
       <c r="J44" s="8">
         <v>2.7566666666666699</v>
       </c>
-      <c r="K44" s="7">
+      <c r="K44" s="8">
+        <f t="shared" si="0"/>
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="L44" s="7">
         <v>97.681629999999998</v>
       </c>
-      <c r="L44" s="8">
+      <c r="M44" s="8">
         <v>0.92339793333333331</v>
       </c>
-      <c r="M44" s="11">
+      <c r="N44" s="11">
         <v>11340148</v>
       </c>
-      <c r="N44" s="10"/>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O44" s="10"/>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A45" s="9">
         <v>39692</v>
       </c>
@@ -8913,18 +9086,22 @@
       <c r="J45" s="8">
         <v>3.0566666666666702</v>
       </c>
-      <c r="K45" s="7">
+      <c r="K45" s="8">
+        <f t="shared" si="0"/>
+        <v>0.80666666666665998</v>
+      </c>
+      <c r="L45" s="7">
         <v>97.669780000000003</v>
       </c>
-      <c r="L45" s="8">
+      <c r="M45" s="8">
         <v>0.9022503666666668</v>
       </c>
-      <c r="M45" s="11">
+      <c r="N45" s="11">
         <v>10812988</v>
       </c>
-      <c r="N45" s="10"/>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O45" s="10"/>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A46" s="9">
         <v>39783</v>
       </c>
@@ -8955,18 +9132,22 @@
       <c r="J46" s="8">
         <v>2.81666666666667</v>
       </c>
-      <c r="K46" s="7">
+      <c r="K46" s="8">
+        <f t="shared" si="0"/>
+        <v>0.43666666666665988</v>
+      </c>
+      <c r="L46" s="7">
         <v>97.022220000000004</v>
       </c>
-      <c r="L46" s="8">
+      <c r="M46" s="8">
         <v>0.89604403333333327</v>
       </c>
-      <c r="M46" s="11">
+      <c r="N46" s="11">
         <v>10342620</v>
       </c>
-      <c r="N46" s="10"/>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O46" s="10"/>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A47" s="9">
         <v>39873</v>
       </c>
@@ -8997,18 +9178,22 @@
       <c r="J47" s="8">
         <v>1.0833333333333299</v>
       </c>
-      <c r="K47" s="7">
+      <c r="K47" s="8">
+        <f t="shared" si="0"/>
+        <v>1.65333333333334</v>
+      </c>
+      <c r="L47" s="7">
         <v>97.196579999999997</v>
       </c>
-      <c r="L47" s="8">
+      <c r="M47" s="8">
         <v>0.90080876666666665</v>
       </c>
-      <c r="M47" s="11">
+      <c r="N47" s="11">
         <v>9816515</v>
       </c>
-      <c r="N47" s="10"/>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O47" s="10"/>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A48" s="9">
         <v>39965</v>
       </c>
@@ -9039,18 +9224,22 @@
       <c r="J48" s="8">
         <v>0.61666666666666703</v>
       </c>
-      <c r="K48" s="7">
+      <c r="K48" s="8">
+        <f t="shared" si="0"/>
+        <v>2.6966666666666628</v>
+      </c>
+      <c r="L48" s="7">
         <v>98.458179999999999</v>
       </c>
-      <c r="L48" s="8">
+      <c r="M48" s="8">
         <v>0.90855929999999996</v>
       </c>
-      <c r="M48" s="11">
+      <c r="N48" s="11">
         <v>9423210</v>
       </c>
-      <c r="N48" s="10"/>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O48" s="10"/>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A49" s="9">
         <v>40057</v>
       </c>
@@ -9081,18 +9270,22 @@
       <c r="J49" s="8">
         <v>0.3</v>
       </c>
-      <c r="K49" s="7">
+      <c r="K49" s="8">
+        <f t="shared" si="0"/>
+        <v>3.2166666666666703</v>
+      </c>
+      <c r="L49" s="7">
         <v>99.113069999999993</v>
       </c>
-      <c r="L49" s="8">
+      <c r="M49" s="8">
         <v>0.91567273333333332</v>
       </c>
-      <c r="M49" s="11">
+      <c r="N49" s="11">
         <v>9171520</v>
       </c>
-      <c r="N49" s="10"/>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O49" s="10"/>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A50" s="9">
         <v>40148</v>
       </c>
@@ -9123,18 +9316,22 @@
       <c r="J50" s="8">
         <v>0.223333333333333</v>
       </c>
-      <c r="K50" s="7">
+      <c r="K50" s="8">
+        <f t="shared" si="0"/>
+        <v>3.2366666666666668</v>
+      </c>
+      <c r="L50" s="7">
         <v>99.300870000000003</v>
       </c>
-      <c r="L50" s="8">
+      <c r="M50" s="8">
         <v>0.91712410000000011</v>
       </c>
-      <c r="M50" s="11">
+      <c r="N50" s="11">
         <v>9001160</v>
       </c>
-      <c r="N50" s="10"/>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O50" s="10"/>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A51" s="9">
         <v>40238</v>
       </c>
@@ -9165,18 +9362,22 @@
       <c r="J51" s="8">
         <v>0.206666666666667</v>
       </c>
-      <c r="K51" s="7">
+      <c r="K51" s="8">
+        <f t="shared" si="0"/>
+        <v>3.5100000000000029</v>
+      </c>
+      <c r="L51" s="7">
         <v>99.382689999999997</v>
       </c>
-      <c r="L51" s="8">
+      <c r="M51" s="8">
         <v>0.91680063333333317</v>
       </c>
-      <c r="M51" s="11">
+      <c r="N51" s="11">
         <v>9029161</v>
       </c>
-      <c r="N51" s="10"/>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O51" s="10"/>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A52" s="9">
         <v>40330</v>
       </c>
@@ -9207,18 +9408,22 @@
       <c r="J52" s="8">
         <v>0.42333333333333301</v>
       </c>
-      <c r="K52" s="7">
+      <c r="K52" s="8">
+        <f t="shared" si="0"/>
+        <v>3.0666666666666673</v>
+      </c>
+      <c r="L52" s="7">
         <v>99.261229999999998</v>
       </c>
-      <c r="L52" s="8">
+      <c r="M52" s="8">
         <v>0.91948819999999998</v>
       </c>
-      <c r="M52" s="11">
+      <c r="N52" s="11">
         <v>9016813</v>
       </c>
-      <c r="N52" s="10"/>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O52" s="10"/>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A53" s="9">
         <v>40422</v>
       </c>
@@ -9249,18 +9454,22 @@
       <c r="J53" s="8">
         <v>0.336666666666667</v>
       </c>
-      <c r="K53" s="7">
+      <c r="K53" s="8">
+        <f t="shared" si="0"/>
+        <v>2.4500000000000033</v>
+      </c>
+      <c r="L53" s="7">
         <v>99.259219999999999</v>
       </c>
-      <c r="L53" s="8">
+      <c r="M53" s="8">
         <v>0.92693349999999997</v>
       </c>
-      <c r="M53" s="11">
+      <c r="N53" s="11">
         <v>8949540</v>
       </c>
-      <c r="N53" s="10"/>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O53" s="10"/>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A54" s="9">
         <v>40513</v>
       </c>
@@ -9291,18 +9500,22 @@
       <c r="J54" s="8">
         <v>0.28000000000000003</v>
       </c>
-      <c r="K54" s="7">
+      <c r="K54" s="8">
+        <f t="shared" si="0"/>
+        <v>2.5833333333333304</v>
+      </c>
+      <c r="L54" s="7">
         <v>99.417169999999999</v>
       </c>
-      <c r="L54" s="8">
+      <c r="M54" s="8">
         <v>0.9368258666666669</v>
       </c>
-      <c r="M54" s="11">
+      <c r="N54" s="11">
         <v>8853863</v>
       </c>
-      <c r="N54" s="10"/>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O54" s="10"/>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A55" s="9">
         <v>40603</v>
       </c>
@@ -9333,18 +9546,22 @@
       <c r="J55" s="8">
         <v>0.28333333333333299</v>
       </c>
-      <c r="K55" s="7">
+      <c r="K55" s="8">
+        <f t="shared" si="0"/>
+        <v>3.1766666666666667</v>
+      </c>
+      <c r="L55" s="7">
         <v>99.039929999999998</v>
       </c>
-      <c r="L55" s="8">
+      <c r="M55" s="8">
         <v>0.94747776666666672</v>
       </c>
-      <c r="M55" s="11">
+      <c r="N55" s="11">
         <v>8562983</v>
       </c>
-      <c r="N55" s="10"/>
-    </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O55" s="10"/>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A56" s="9">
         <v>40695</v>
       </c>
@@ -9375,18 +9592,22 @@
       <c r="J56" s="8">
         <v>0.22</v>
       </c>
-      <c r="K56" s="7">
+      <c r="K56" s="8">
+        <f t="shared" si="0"/>
+        <v>2.9899999999999998</v>
+      </c>
+      <c r="L56" s="7">
         <v>98.816429999999997</v>
       </c>
-      <c r="L56" s="8">
+      <c r="M56" s="8">
         <v>0.95365593333333321</v>
       </c>
-      <c r="M56" s="11">
+      <c r="N56" s="11">
         <v>8515245</v>
       </c>
-      <c r="N56" s="10"/>
-    </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O56" s="10"/>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A57" s="9">
         <v>40787</v>
       </c>
@@ -9417,18 +9638,22 @@
       <c r="J57" s="8">
         <v>0.28666666666666701</v>
       </c>
-      <c r="K57" s="7">
+      <c r="K57" s="8">
+        <f t="shared" si="0"/>
+        <v>2.1400000000000028</v>
+      </c>
+      <c r="L57" s="7">
         <v>98.1952</v>
       </c>
-      <c r="L57" s="8">
+      <c r="M57" s="8">
         <v>0.95793689999999998</v>
       </c>
-      <c r="M57" s="11">
+      <c r="N57" s="11">
         <v>8482046</v>
       </c>
-      <c r="N57" s="10"/>
-    </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O57" s="10"/>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A58" s="9">
         <v>40878</v>
       </c>
@@ -9459,18 +9684,22 @@
       <c r="J58" s="8">
         <v>0.42333333333333301</v>
       </c>
-      <c r="K58" s="7">
+      <c r="K58" s="8">
+        <f t="shared" si="0"/>
+        <v>1.6233333333333371</v>
+      </c>
+      <c r="L58" s="7">
         <v>98.532120000000006</v>
       </c>
-      <c r="L58" s="8">
+      <c r="M58" s="8">
         <v>0.96333173333333333</v>
       </c>
-      <c r="M58" s="11">
+      <c r="N58" s="11">
         <v>8366789.0000000009</v>
       </c>
-      <c r="N58" s="10"/>
-    </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O58" s="10"/>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A59" s="9">
         <v>40969</v>
       </c>
@@ -9501,18 +9730,22 @@
       <c r="J59" s="8">
         <v>0.33</v>
       </c>
-      <c r="K59" s="7">
+      <c r="K59" s="8">
+        <f t="shared" si="0"/>
+        <v>1.7066666666666701</v>
+      </c>
+      <c r="L59" s="7">
         <v>98.951620000000005</v>
       </c>
-      <c r="L59" s="8">
+      <c r="M59" s="8">
         <v>0.96536533333333319</v>
       </c>
-      <c r="M59" s="11">
+      <c r="N59" s="11">
         <v>8247222</v>
       </c>
-      <c r="N59" s="10"/>
-    </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O59" s="10"/>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A60" s="9">
         <v>41061</v>
       </c>
@@ -9543,18 +9776,22 @@
       <c r="J60" s="8">
         <v>0.3</v>
       </c>
-      <c r="K60" s="7">
+      <c r="K60" s="8">
+        <f t="shared" si="0"/>
+        <v>1.5233333333333299</v>
+      </c>
+      <c r="L60" s="7">
         <v>98.822659999999999</v>
       </c>
-      <c r="L60" s="8">
+      <c r="M60" s="8">
         <v>0.96972369999999997</v>
       </c>
-      <c r="M60" s="11">
+      <c r="N60" s="11">
         <v>8500254</v>
       </c>
-      <c r="N60" s="10"/>
-    </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O60" s="10"/>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A61" s="9">
         <v>41153</v>
       </c>
@@ -9585,18 +9822,22 @@
       <c r="J61" s="8">
         <v>0.266666666666667</v>
       </c>
-      <c r="K61" s="7">
+      <c r="K61" s="8">
+        <f t="shared" si="0"/>
+        <v>1.3766666666666629</v>
+      </c>
+      <c r="L61" s="7">
         <v>98.816770000000005</v>
       </c>
-      <c r="L61" s="8">
+      <c r="M61" s="8">
         <v>0.97617189999999998</v>
       </c>
-      <c r="M61" s="11">
+      <c r="N61" s="11">
         <v>8789833</v>
       </c>
-      <c r="N61" s="10"/>
-    </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O61" s="10"/>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A62" s="9">
         <v>41244</v>
       </c>
@@ -9627,18 +9868,22 @@
       <c r="J62" s="8">
         <v>0.233333333333333</v>
       </c>
-      <c r="K62" s="7">
+      <c r="K62" s="8">
+        <f t="shared" si="0"/>
+        <v>1.4733333333333372</v>
+      </c>
+      <c r="L62" s="7">
         <v>98.836569999999995</v>
       </c>
-      <c r="L62" s="8">
+      <c r="M62" s="8">
         <v>0.98009563333333327</v>
       </c>
-      <c r="M62" s="11">
+      <c r="N62" s="11">
         <v>9025529</v>
       </c>
-      <c r="N62" s="10"/>
-    </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O62" s="10"/>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A63" s="9">
         <v>41334</v>
       </c>
@@ -9669,18 +9914,22 @@
       <c r="J63" s="8">
         <v>0.22</v>
       </c>
-      <c r="K63" s="7">
+      <c r="K63" s="8">
+        <f t="shared" si="0"/>
+        <v>1.73</v>
+      </c>
+      <c r="L63" s="7">
         <v>99.129459999999995</v>
       </c>
-      <c r="L63" s="8">
+      <c r="M63" s="8">
         <v>0.97902256666666654</v>
       </c>
-      <c r="M63" s="11">
+      <c r="N63" s="11">
         <v>9484169</v>
       </c>
-      <c r="N63" s="10"/>
-    </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O63" s="10"/>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A64" s="9">
         <v>41426</v>
       </c>
@@ -9711,18 +9960,22 @@
       <c r="J64" s="8">
         <v>0.19666666666666699</v>
       </c>
-      <c r="K64" s="7">
+      <c r="K64" s="8">
+        <f t="shared" si="0"/>
+        <v>1.8000000000000029</v>
+      </c>
+      <c r="L64" s="7">
         <v>99.511259999999993</v>
       </c>
-      <c r="L64" s="8">
+      <c r="M64" s="8">
         <v>0.9843175666666667</v>
       </c>
-      <c r="M64" s="11">
+      <c r="N64" s="11">
         <v>10022483</v>
       </c>
-      <c r="N64" s="10"/>
-    </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O64" s="10"/>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A65" s="9">
         <v>41518</v>
       </c>
@@ -9753,18 +10006,22 @@
       <c r="J65" s="8">
         <v>0.123333333333333</v>
       </c>
-      <c r="K65" s="7">
+      <c r="K65" s="8">
+        <f t="shared" si="0"/>
+        <v>2.5866666666666669</v>
+      </c>
+      <c r="L65" s="7">
         <v>99.576809999999995</v>
       </c>
-      <c r="L65" s="8">
+      <c r="M65" s="8">
         <v>0.98795726666666672</v>
       </c>
-      <c r="M65" s="11">
+      <c r="N65" s="11">
         <v>10531175</v>
       </c>
-      <c r="N65" s="10"/>
-    </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O65" s="10"/>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A66" s="9">
         <v>41609</v>
       </c>
@@ -9795,18 +10052,22 @@
       <c r="J66" s="8">
         <v>0.12666666666666701</v>
       </c>
-      <c r="K66" s="7">
+      <c r="K66" s="8">
+        <f t="shared" si="0"/>
+        <v>2.6200000000000032</v>
+      </c>
+      <c r="L66" s="7">
         <v>99.617099999999994</v>
       </c>
-      <c r="L66" s="8">
+      <c r="M66" s="8">
         <v>0.9941101333333332</v>
       </c>
-      <c r="M66" s="11">
+      <c r="N66" s="11">
         <v>10887599</v>
       </c>
-      <c r="N66" s="10"/>
-    </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O66" s="10"/>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A67" s="9">
         <v>41699</v>
       </c>
@@ -9837,18 +10098,22 @@
       <c r="J67" s="8">
         <v>0.123333333333333</v>
       </c>
-      <c r="K67" s="7">
+      <c r="K67" s="8">
+        <f t="shared" ref="K67:K106" si="1">I67-J67</f>
+        <v>2.639999999999997</v>
+      </c>
+      <c r="L67" s="7">
         <v>99.805719999999994</v>
       </c>
-      <c r="L67" s="8">
+      <c r="M67" s="8">
         <v>0.99938966666666662</v>
       </c>
-      <c r="M67" s="11">
+      <c r="N67" s="11">
         <v>11224669</v>
       </c>
-      <c r="N67" s="10"/>
-    </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O67" s="10"/>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A68" s="9">
         <v>41791</v>
       </c>
@@ -9879,18 +10144,22 @@
       <c r="J68" s="8">
         <v>0.11333333333333299</v>
       </c>
-      <c r="K68" s="7">
+      <c r="K68" s="8">
+        <f t="shared" si="1"/>
+        <v>2.5099999999999971</v>
+      </c>
+      <c r="L68" s="7">
         <v>99.978549999999998</v>
       </c>
-      <c r="L68" s="8">
+      <c r="M68" s="8">
         <v>1.0019463333333329</v>
       </c>
-      <c r="M68" s="11">
+      <c r="N68" s="11">
         <v>11667975</v>
       </c>
-      <c r="N68" s="10"/>
-    </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O68" s="10"/>
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A69" s="9">
         <v>41883</v>
       </c>
@@ -9921,18 +10190,22 @@
       <c r="J69" s="8">
         <v>0.12666666666666701</v>
       </c>
-      <c r="K69" s="7">
+      <c r="K69" s="8">
+        <f t="shared" si="1"/>
+        <v>2.3700000000000032</v>
+      </c>
+      <c r="L69" s="7">
         <v>99.949150000000003</v>
       </c>
-      <c r="L69" s="8">
+      <c r="M69" s="8">
         <v>0.99945700000000004</v>
       </c>
-      <c r="M69" s="11">
+      <c r="N69" s="11">
         <v>12055342</v>
       </c>
-      <c r="N69" s="10"/>
-    </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O69" s="10"/>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A70" s="9">
         <v>41974</v>
       </c>
@@ -9963,18 +10236,22 @@
       <c r="J70" s="8">
         <v>0.133333333333333</v>
       </c>
-      <c r="K70" s="7">
+      <c r="K70" s="8">
+        <f t="shared" si="1"/>
+        <v>2.1466666666666669</v>
+      </c>
+      <c r="L70" s="7">
         <v>100.2978</v>
       </c>
-      <c r="L70" s="8">
+      <c r="M70" s="8">
         <v>0.99298783333333329</v>
       </c>
-      <c r="M70" s="11">
+      <c r="N70" s="11">
         <v>12300063</v>
       </c>
-      <c r="N70" s="10"/>
-    </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O70" s="10"/>
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A71" s="9">
         <v>42064</v>
       </c>
@@ -10005,18 +10282,22 @@
       <c r="J71" s="8">
         <v>0.15</v>
       </c>
-      <c r="K71" s="7">
+      <c r="K71" s="8">
+        <f t="shared" si="1"/>
+        <v>1.81666666666667</v>
+      </c>
+      <c r="L71" s="7">
         <v>100.6968</v>
       </c>
-      <c r="L71" s="8">
+      <c r="M71" s="8">
         <v>0.99975943333333328</v>
       </c>
-      <c r="M71" s="11">
+      <c r="N71" s="11">
         <v>12663787</v>
       </c>
-      <c r="N71" s="10"/>
-    </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O71" s="10"/>
+    </row>
+    <row r="72" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A72" s="9">
         <v>42156</v>
       </c>
@@ -10047,18 +10328,22 @@
       <c r="J72" s="8">
         <v>0.15333333333333299</v>
       </c>
-      <c r="K72" s="7">
+      <c r="K72" s="8">
+        <f t="shared" si="1"/>
+        <v>2.0133333333333372</v>
+      </c>
+      <c r="L72" s="7">
         <v>100.57599999999999</v>
       </c>
-      <c r="L72" s="8">
+      <c r="M72" s="8">
         <v>1.003535666666667</v>
       </c>
-      <c r="M72" s="11">
+      <c r="N72" s="11">
         <v>13074415</v>
       </c>
-      <c r="N72" s="10"/>
-    </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O72" s="10"/>
+    </row>
+    <row r="73" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A73" s="9">
         <v>42248</v>
       </c>
@@ -10089,18 +10374,22 @@
       <c r="J73" s="8">
         <v>0.24</v>
       </c>
-      <c r="K73" s="7">
+      <c r="K73" s="8">
+        <f t="shared" si="1"/>
+        <v>1.9800000000000002</v>
+      </c>
+      <c r="L73" s="7">
         <v>100.3537</v>
       </c>
-      <c r="L73" s="8">
+      <c r="M73" s="8">
         <v>1.0034596666666671</v>
       </c>
-      <c r="M73" s="11">
+      <c r="N73" s="11">
         <v>13473214</v>
       </c>
-      <c r="N73" s="10"/>
-    </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O73" s="10"/>
+    </row>
+    <row r="74" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A74" s="9">
         <v>42339</v>
       </c>
@@ -10131,18 +10420,22 @@
       <c r="J74" s="8">
         <v>0.36333333333333301</v>
       </c>
-      <c r="K74" s="7">
+      <c r="K74" s="8">
+        <f t="shared" si="1"/>
+        <v>1.8266666666666669</v>
+      </c>
+      <c r="L74" s="7">
         <v>100.64239999999999</v>
       </c>
-      <c r="L74" s="8">
+      <c r="M74" s="8">
         <v>1.002836666666667</v>
       </c>
-      <c r="M74" s="11">
+      <c r="N74" s="11">
         <v>13739108</v>
       </c>
-      <c r="N74" s="10"/>
-    </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O74" s="10"/>
+    </row>
+    <row r="75" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A75" s="9">
         <v>42430</v>
       </c>
@@ -10173,18 +10466,22 @@
       <c r="J75" s="8">
         <v>0.55333333333333301</v>
       </c>
-      <c r="K75" s="7">
+      <c r="K75" s="8">
+        <f t="shared" si="1"/>
+        <v>1.3666666666666669</v>
+      </c>
+      <c r="L75" s="7">
         <v>100.4003</v>
       </c>
-      <c r="L75" s="8">
+      <c r="M75" s="8">
         <v>1.0108573333333331</v>
       </c>
-      <c r="M75" s="11">
+      <c r="N75" s="11">
         <v>14030997</v>
       </c>
-      <c r="N75" s="10"/>
-    </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O75" s="10"/>
+    </row>
+    <row r="76" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A76" s="9">
         <v>42522</v>
       </c>
@@ -10215,18 +10512,22 @@
       <c r="J76" s="8">
         <v>0.55666666666666698</v>
       </c>
-      <c r="K76" s="7">
+      <c r="K76" s="8">
+        <f t="shared" si="1"/>
+        <v>1.1966666666666632</v>
+      </c>
+      <c r="L76" s="7">
         <v>100.4448</v>
       </c>
-      <c r="L76" s="8">
+      <c r="M76" s="8">
         <v>1.0151479999999999</v>
       </c>
-      <c r="M76" s="11">
+      <c r="N76" s="11">
         <v>14515384</v>
       </c>
-      <c r="N76" s="10"/>
-    </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O76" s="10"/>
+    </row>
+    <row r="77" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A77" s="9">
         <v>42614</v>
       </c>
@@ -10257,18 +10558,22 @@
       <c r="J77" s="8">
         <v>0.7</v>
       </c>
-      <c r="K77" s="7">
+      <c r="K77" s="8">
+        <f t="shared" si="1"/>
+        <v>0.86333333333332996</v>
+      </c>
+      <c r="L77" s="7">
         <v>100.38500000000001</v>
       </c>
-      <c r="L77" s="8">
+      <c r="M77" s="8">
         <v>1.0215916666666671</v>
       </c>
-      <c r="M77" s="11">
+      <c r="N77" s="11">
         <v>14951477</v>
       </c>
-      <c r="N77" s="10"/>
-    </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O77" s="10"/>
+    </row>
+    <row r="78" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A78" s="9">
         <v>42705</v>
       </c>
@@ -10299,18 +10604,22 @@
       <c r="J78" s="8">
         <v>0.76666666666666605</v>
       </c>
-      <c r="K78" s="7">
+      <c r="K78" s="8">
+        <f t="shared" si="1"/>
+        <v>1.3633333333333337</v>
+      </c>
+      <c r="L78" s="7">
         <v>100.55110000000001</v>
       </c>
-      <c r="L78" s="8">
+      <c r="M78" s="8">
         <v>1.0287809999999999</v>
       </c>
-      <c r="M78" s="11">
+      <c r="N78" s="11">
         <v>15306835</v>
       </c>
-      <c r="N78" s="10"/>
-    </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O78" s="10"/>
+    </row>
+    <row r="79" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A79" s="9">
         <v>42795</v>
       </c>
@@ -10341,18 +10650,22 @@
       <c r="J79" s="8">
         <v>0.91666666666666596</v>
       </c>
-      <c r="K79" s="7">
+      <c r="K79" s="8">
+        <f t="shared" si="1"/>
+        <v>1.5266666666666637</v>
+      </c>
+      <c r="L79" s="7">
         <v>100.6679</v>
       </c>
-      <c r="L79" s="8">
+      <c r="M79" s="8">
         <v>1.0299683333333329</v>
       </c>
-      <c r="M79" s="11">
+      <c r="N79" s="11">
         <v>15677410</v>
       </c>
-      <c r="N79" s="10"/>
-    </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O79" s="10"/>
+    </row>
+    <row r="80" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A80" s="9">
         <v>42887</v>
       </c>
@@ -10383,18 +10696,22 @@
       <c r="J80" s="8">
         <v>1.08</v>
       </c>
-      <c r="K80" s="7">
+      <c r="K80" s="8">
+        <f t="shared" si="1"/>
+        <v>1.18333333333333</v>
+      </c>
+      <c r="L80" s="7">
         <v>100.86879999999999</v>
       </c>
-      <c r="L80" s="8">
+      <c r="M80" s="8">
         <v>1.0348919999999999</v>
       </c>
-      <c r="M80" s="11">
+      <c r="N80" s="11">
         <v>16132392</v>
       </c>
-      <c r="N80" s="10"/>
-    </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O80" s="10"/>
+    </row>
+    <row r="81" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A81" s="9">
         <v>42979</v>
       </c>
@@ -10425,18 +10742,22 @@
       <c r="J81" s="8">
         <v>1.24</v>
       </c>
-      <c r="K81" s="7">
+      <c r="K81" s="8">
+        <f t="shared" si="1"/>
+        <v>1.0033333333333301</v>
+      </c>
+      <c r="L81" s="7">
         <v>101.0384</v>
       </c>
-      <c r="L81" s="8">
+      <c r="M81" s="8">
         <v>1.0431250000000001</v>
       </c>
-      <c r="M81" s="11">
+      <c r="N81" s="11">
         <v>16557733</v>
       </c>
-      <c r="N81" s="10"/>
-    </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O81" s="10"/>
+    </row>
+    <row r="82" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A82" s="9">
         <v>43070</v>
       </c>
@@ -10467,18 +10788,22 @@
       <c r="J82" s="8">
         <v>1.37333333333333</v>
       </c>
-      <c r="K82" s="7">
+      <c r="K82" s="8">
+        <f t="shared" si="1"/>
+        <v>0.99666666666667014</v>
+      </c>
+      <c r="L82" s="7">
         <v>101.145</v>
       </c>
-      <c r="L82" s="8">
+      <c r="M82" s="8">
         <v>1.051914666666667</v>
       </c>
-      <c r="M82" s="11">
+      <c r="N82" s="11">
         <v>16887561</v>
       </c>
-      <c r="N82" s="10"/>
-    </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O82" s="10"/>
+    </row>
+    <row r="83" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A83" s="9">
         <v>43160</v>
       </c>
@@ -10509,18 +10834,22 @@
       <c r="J83" s="8">
         <v>1.83</v>
       </c>
-      <c r="K83" s="7">
+      <c r="K83" s="8">
+        <f t="shared" si="1"/>
+        <v>0.92999999999999972</v>
+      </c>
+      <c r="L83" s="7">
         <v>101.169</v>
       </c>
-      <c r="L83" s="8">
+      <c r="M83" s="8">
         <v>1.057641333333333</v>
       </c>
-      <c r="M83" s="11">
+      <c r="N83" s="11">
         <v>17476639</v>
       </c>
-      <c r="N83" s="10"/>
-    </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O83" s="10"/>
+    </row>
+    <row r="84" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A84" s="9">
         <v>43252</v>
       </c>
@@ -10551,18 +10880,22 @@
       <c r="J84" s="8">
         <v>2.18333333333333</v>
       </c>
-      <c r="K84" s="7">
+      <c r="K84" s="8">
+        <f t="shared" si="1"/>
+        <v>0.73666666666666991</v>
+      </c>
+      <c r="L84" s="7">
         <v>101.16289999999999</v>
       </c>
-      <c r="L84" s="8">
+      <c r="M84" s="8">
         <v>1.0618916666666669</v>
       </c>
-      <c r="M84" s="11">
+      <c r="N84" s="11">
         <v>17791049</v>
       </c>
-      <c r="N84" s="10"/>
-    </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O84" s="10"/>
+    </row>
+    <row r="85" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A85" s="9">
         <v>43344</v>
       </c>
@@ -10593,18 +10926,22 @@
       <c r="J85" s="8">
         <v>2.2000000000000002</v>
       </c>
-      <c r="K85" s="7">
+      <c r="K85" s="8">
+        <f t="shared" si="1"/>
+        <v>0.72666666666666968</v>
+      </c>
+      <c r="L85" s="7">
         <v>101.0658</v>
       </c>
-      <c r="L85" s="8">
+      <c r="M85" s="8">
         <v>1.066214666666667</v>
       </c>
-      <c r="M85" s="11">
+      <c r="N85" s="11">
         <v>18053819</v>
       </c>
-      <c r="N85" s="10"/>
-    </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O85" s="10"/>
+    </row>
+    <row r="86" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A86" s="9">
         <v>43435</v>
       </c>
@@ -10635,18 +10972,22 @@
       <c r="J86" s="8">
         <v>2.54</v>
       </c>
-      <c r="K86" s="7">
+      <c r="K86" s="8">
+        <f t="shared" si="1"/>
+        <v>0.49333333333333007</v>
+      </c>
+      <c r="L86" s="7">
         <v>100.7903</v>
       </c>
-      <c r="L86" s="8">
+      <c r="M86" s="8">
         <v>1.069061333333333</v>
       </c>
-      <c r="M86" s="11">
+      <c r="N86" s="11">
         <v>18262497</v>
       </c>
-      <c r="N86" s="10"/>
-    </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O86" s="10"/>
+    </row>
+    <row r="87" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A87" s="9">
         <v>43525</v>
       </c>
@@ -10677,18 +11018,22 @@
       <c r="J87" s="8">
         <v>2.52</v>
       </c>
-      <c r="K87" s="7">
+      <c r="K87" s="8">
+        <f t="shared" si="1"/>
+        <v>0.1333333333333302</v>
+      </c>
+      <c r="L87" s="7">
         <v>100.9063</v>
       </c>
-      <c r="L87" s="8">
+      <c r="M87" s="8">
         <v>1.076915666666667</v>
       </c>
-      <c r="M87" s="11">
+      <c r="N87" s="11">
         <v>18729124</v>
       </c>
-      <c r="N87" s="10"/>
-    </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O87" s="10"/>
+    </row>
+    <row r="88" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A88" s="9">
         <v>43617</v>
       </c>
@@ -10719,18 +11064,22 @@
       <c r="J88" s="8">
         <v>2.4033333333333302</v>
       </c>
-      <c r="K88" s="7">
+      <c r="K88" s="8">
+        <f t="shared" si="1"/>
+        <v>-7.0000000000000284E-2</v>
+      </c>
+      <c r="L88" s="7">
         <v>100.7931</v>
       </c>
-      <c r="L88" s="8">
+      <c r="M88" s="8">
         <v>1.0804683333333329</v>
       </c>
-      <c r="M88" s="11">
+      <c r="N88" s="11">
         <v>19022630</v>
       </c>
-      <c r="N88" s="10"/>
-    </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O88" s="10"/>
+    </row>
+    <row r="89" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A89" s="9">
         <v>43709</v>
       </c>
@@ -10761,18 +11110,22 @@
       <c r="J89" s="8">
         <v>2.1033333333333299</v>
       </c>
-      <c r="K89" s="7">
+      <c r="K89" s="8">
+        <f t="shared" si="1"/>
+        <v>-0.30666666666665998</v>
+      </c>
+      <c r="L89" s="7">
         <v>100.4945</v>
       </c>
-      <c r="L89" s="8">
+      <c r="M89" s="8">
         <v>1.0880570000000001</v>
       </c>
-      <c r="M89" s="11">
+      <c r="N89" s="11">
         <v>19220225</v>
       </c>
-      <c r="N89" s="10"/>
-    </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O89" s="10"/>
+    </row>
+    <row r="90" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A90" s="9">
         <v>43800</v>
       </c>
@@ -10803,18 +11156,22 @@
       <c r="J90" s="8">
         <v>1.8033333333333299</v>
       </c>
-      <c r="K90" s="7">
+      <c r="K90" s="8">
+        <f t="shared" si="1"/>
+        <v>-1.0000000000000009E-2</v>
+      </c>
+      <c r="L90" s="7">
         <v>100.8145</v>
       </c>
-      <c r="L90" s="8">
+      <c r="M90" s="8">
         <v>1.091979</v>
       </c>
-      <c r="M90" s="11">
+      <c r="N90" s="11">
         <v>19499628</v>
       </c>
-      <c r="N90" s="10"/>
-    </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O90" s="10"/>
+    </row>
+    <row r="91" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A91" s="9">
         <v>43891</v>
       </c>
@@ -10845,18 +11202,22 @@
       <c r="J91" s="8">
         <v>1.53</v>
       </c>
-      <c r="K91" s="7">
+      <c r="K91" s="8">
+        <f t="shared" si="1"/>
+        <v>-0.15333333333332999</v>
+      </c>
+      <c r="L91" s="7">
         <v>99.213660000000004</v>
       </c>
-      <c r="L91" s="8">
+      <c r="M91" s="8">
         <v>1.081323333333333</v>
       </c>
-      <c r="M91" s="11">
+      <c r="N91" s="11">
         <v>20107785</v>
       </c>
-      <c r="N91" s="10"/>
-    </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O91" s="10"/>
+    </row>
+    <row r="92" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A92" s="9">
         <v>43983</v>
       </c>
@@ -10887,18 +11248,22 @@
       <c r="J92" s="8">
         <v>0.185</v>
       </c>
-      <c r="K92" s="7">
+      <c r="K92" s="8">
+        <f t="shared" si="1"/>
+        <v>0.50166666666666693</v>
+      </c>
+      <c r="L92" s="7">
         <v>97.955550000000002</v>
       </c>
-      <c r="L92" s="8">
+      <c r="M92" s="8">
         <v>1.0936839999999999</v>
       </c>
-      <c r="M92" s="11">
+      <c r="N92" s="11">
         <v>20778502</v>
       </c>
-      <c r="N92" s="10"/>
-    </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O92" s="10"/>
+    </row>
+    <row r="93" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A93" s="9">
         <v>44075</v>
       </c>
@@ -10929,18 +11294,22 @@
       <c r="J93" s="8">
         <v>0.15333333333333299</v>
       </c>
-      <c r="K93" s="7">
+      <c r="K93" s="8">
+        <f t="shared" si="1"/>
+        <v>0.49666666666666703</v>
+      </c>
+      <c r="L93" s="7">
         <v>98.700329999999994</v>
       </c>
-      <c r="L93" s="8">
+      <c r="M93" s="8">
         <v>1.1015736666666671</v>
       </c>
-      <c r="M93" s="11">
+      <c r="N93" s="11">
         <v>21397548</v>
       </c>
-      <c r="N93" s="10"/>
-    </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O93" s="10"/>
+    </row>
+    <row r="94" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A94" s="9">
         <v>44166</v>
       </c>
@@ -10971,18 +11340,22 @@
       <c r="J94" s="8">
         <v>0.15</v>
       </c>
-      <c r="K94" s="7">
+      <c r="K94" s="8">
+        <f t="shared" si="1"/>
+        <v>0.71333333333333393</v>
+      </c>
+      <c r="L94" s="7">
         <v>98.909030000000001</v>
       </c>
-      <c r="L94" s="8">
+      <c r="M94" s="8">
         <v>1.1125210000000001</v>
       </c>
-      <c r="M94" s="11">
+      <c r="N94" s="11">
         <v>22226133</v>
       </c>
-      <c r="N94" s="10"/>
-    </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O94" s="10"/>
+    </row>
+    <row r="95" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A95" s="9">
         <v>44256</v>
       </c>
@@ -11013,18 +11386,22 @@
       <c r="J95" s="8">
         <v>0.116666666666667</v>
       </c>
-      <c r="K95" s="7">
+      <c r="K95" s="8">
+        <f t="shared" si="1"/>
+        <v>1.2000000000000031</v>
+      </c>
+      <c r="L95" s="7">
         <v>99.730770000000007</v>
       </c>
-      <c r="L95" s="8">
+      <c r="M95" s="8">
         <v>1.1331659999999999</v>
       </c>
-      <c r="M95" s="11">
+      <c r="N95" s="11">
         <v>23402509</v>
       </c>
-      <c r="N95" s="10"/>
-    </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O95" s="10"/>
+    </row>
+    <row r="96" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A96" s="9">
         <v>44348</v>
       </c>
@@ -11055,18 +11432,22 @@
       <c r="J96" s="8">
         <v>0.1</v>
       </c>
-      <c r="K96" s="7">
+      <c r="K96" s="8">
+        <f t="shared" si="1"/>
+        <v>1.4933333333333298</v>
+      </c>
+      <c r="L96" s="7">
         <v>100.4494</v>
       </c>
-      <c r="L96" s="8">
+      <c r="M96" s="8">
         <v>1.1513363333333329</v>
       </c>
-      <c r="M96" s="11">
+      <c r="N96" s="11">
         <v>25141129</v>
       </c>
-      <c r="N96" s="10"/>
-    </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O96" s="10"/>
+    </row>
+    <row r="97" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A97" s="9">
         <v>44440</v>
       </c>
@@ -11097,18 +11478,22 @@
       <c r="J97" s="8">
         <v>0.1</v>
       </c>
-      <c r="K97" s="7">
+      <c r="K97" s="8">
+        <f t="shared" si="1"/>
+        <v>1.2233333333333298</v>
+      </c>
+      <c r="L97" s="7">
         <v>99.94838</v>
       </c>
-      <c r="L97" s="8">
+      <c r="M97" s="8">
         <v>1.1759463333333331</v>
       </c>
-      <c r="M97" s="11">
+      <c r="N97" s="11">
         <v>26624472</v>
       </c>
-      <c r="N97" s="10"/>
-    </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O97" s="10"/>
+    </row>
+    <row r="98" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A98" s="9">
         <v>44531</v>
       </c>
@@ -11139,18 +11524,22 @@
       <c r="J98" s="8">
         <v>0.14000000000000001</v>
       </c>
-      <c r="K98" s="7">
+      <c r="K98" s="8">
+        <f t="shared" si="1"/>
+        <v>1.3966666666666701</v>
+      </c>
+      <c r="L98" s="7">
         <v>99.302250000000001</v>
       </c>
-      <c r="L98" s="8">
+      <c r="M98" s="8">
         <v>1.2017899999999999</v>
       </c>
-      <c r="M98" s="11">
+      <c r="N98" s="11">
         <v>27102471</v>
       </c>
-      <c r="N98" s="10"/>
-    </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O98" s="10"/>
+    </row>
+    <row r="99" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A99" s="9">
         <v>44621</v>
       </c>
@@ -11181,18 +11570,22 @@
       <c r="J99" s="8">
         <v>0.44333333333333302</v>
       </c>
-      <c r="K99" s="7">
+      <c r="K99" s="8">
+        <f t="shared" si="1"/>
+        <v>1.496666666666667</v>
+      </c>
+      <c r="L99" s="7">
         <v>97.961399999999998</v>
       </c>
-      <c r="L99" s="8">
+      <c r="M99" s="8">
         <v>1.2305066666666671</v>
       </c>
-      <c r="M99" s="11">
+      <c r="N99" s="11">
         <v>30505956</v>
       </c>
-      <c r="N99" s="10"/>
-    </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O99" s="10"/>
+    </row>
+    <row r="100" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A100" s="9">
         <v>44713</v>
       </c>
@@ -11223,18 +11616,22 @@
       <c r="J100" s="8">
         <v>1.37</v>
       </c>
-      <c r="K100" s="7">
+      <c r="K100" s="8">
+        <f t="shared" si="1"/>
+        <v>1.56</v>
+      </c>
+      <c r="L100" s="7">
         <v>96.822789999999998</v>
       </c>
-      <c r="L100" s="8">
+      <c r="M100" s="8">
         <v>1.2467783333333329</v>
       </c>
-      <c r="M100" s="11">
+      <c r="N100" s="11">
         <v>32528089</v>
       </c>
-      <c r="N100" s="10"/>
-    </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O100" s="10"/>
+    </row>
+    <row r="101" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A101" s="9">
         <v>44805</v>
       </c>
@@ -11265,18 +11662,22 @@
       <c r="J101" s="8">
         <v>2.8233333333333301</v>
       </c>
-      <c r="K101" s="7">
+      <c r="K101" s="8">
+        <f t="shared" si="1"/>
+        <v>0.28333333333333988</v>
+      </c>
+      <c r="L101" s="7">
         <v>96.657759999999996</v>
       </c>
-      <c r="L101" s="8">
+      <c r="M101" s="8">
         <v>1.2593963333333331</v>
       </c>
-      <c r="M101" s="11">
+      <c r="N101" s="11">
         <v>31022918</v>
       </c>
-      <c r="N101" s="10"/>
-    </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O101" s="10"/>
+    </row>
+    <row r="102" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A102" s="9">
         <v>44896</v>
       </c>
@@ -11307,18 +11708,22 @@
       <c r="J102" s="8">
         <v>4.2733333333333299</v>
       </c>
-      <c r="K102" s="7">
+      <c r="K102" s="8">
+        <f t="shared" si="1"/>
+        <v>-0.4433333333333298</v>
+      </c>
+      <c r="L102" s="7">
         <v>97.212389999999999</v>
       </c>
-      <c r="L102" s="8">
+      <c r="M102" s="8">
         <v>1.270759666666667</v>
       </c>
-      <c r="M102" s="11">
+      <c r="N102" s="11">
         <v>29952110</v>
       </c>
-      <c r="N102" s="10"/>
-    </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O102" s="10"/>
+    </row>
+    <row r="103" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A103" s="9">
         <v>44986</v>
       </c>
@@ -11349,18 +11754,22 @@
       <c r="J103" s="8">
         <v>4.7533333333333303</v>
       </c>
-      <c r="K103" s="7">
+      <c r="K103" s="8">
+        <f t="shared" si="1"/>
+        <v>-1.1066666666666602</v>
+      </c>
+      <c r="L103" s="7">
         <v>97.925510000000003</v>
       </c>
-      <c r="L103" s="8">
+      <c r="M103" s="8">
         <v>1.2801796666666669</v>
       </c>
-      <c r="M103" s="11">
+      <c r="N103" s="11">
         <v>29836816</v>
       </c>
-      <c r="N103" s="10"/>
-    </row>
-    <row r="104" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O103" s="10"/>
+    </row>
+    <row r="104" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A104" s="9">
         <v>45078</v>
       </c>
@@ -11391,18 +11800,22 @@
       <c r="J104" s="8">
         <v>5.1333333333333302</v>
       </c>
-      <c r="K104" s="7">
+      <c r="K104" s="8">
+        <f t="shared" si="1"/>
+        <v>-1.54</v>
+      </c>
+      <c r="L104" s="7">
         <v>98.493570000000005</v>
       </c>
-      <c r="L104" s="8">
+      <c r="M104" s="8">
         <v>1.291225333333333</v>
       </c>
-      <c r="M104" s="11">
+      <c r="N104" s="11">
         <v>31959540</v>
       </c>
-      <c r="N104" s="10"/>
-    </row>
-    <row r="105" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O104" s="10"/>
+    </row>
+    <row r="105" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A105" s="9">
         <v>45170</v>
       </c>
@@ -11433,18 +11846,22 @@
       <c r="J105" s="8">
         <v>5.4266666666666703</v>
       </c>
-      <c r="K105" s="7">
+      <c r="K105" s="8">
+        <f t="shared" si="1"/>
+        <v>-1.2766666666666699</v>
+      </c>
+      <c r="L105" s="7">
         <v>98.322500000000005</v>
       </c>
-      <c r="L105" s="8">
+      <c r="M105" s="8">
         <v>1.3001529999999999</v>
       </c>
-      <c r="M105" s="11">
+      <c r="N105" s="11">
         <v>32347219</v>
       </c>
-      <c r="N105" s="10"/>
-    </row>
-    <row r="106" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O105" s="10"/>
+    </row>
+    <row r="106" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A106" s="9">
         <v>45261</v>
       </c>
@@ -11475,18 +11892,22 @@
       <c r="J106" s="8">
         <v>5.3966666666666674</v>
       </c>
-      <c r="K106" s="7">
+      <c r="K106" s="8">
+        <f t="shared" si="1"/>
+        <v>-0.956666666666667</v>
+      </c>
+      <c r="L106" s="7">
         <v>98.658500000000004</v>
       </c>
-      <c r="L106" s="8">
+      <c r="M106" s="8">
         <v>1.3120339999999999</v>
       </c>
-      <c r="M106" s="11">
+      <c r="N106" s="11">
         <v>31886641</v>
       </c>
-      <c r="N106" s="10"/>
-    </row>
-    <row r="107" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O106" s="10"/>
+    </row>
+    <row r="107" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A107" s="9"/>
       <c r="B107" s="7"/>
       <c r="C107" s="7"/>
@@ -11497,12 +11918,13 @@
       <c r="H107" s="8"/>
       <c r="I107" s="8"/>
       <c r="J107" s="8"/>
-      <c r="K107" s="7"/>
-      <c r="L107" s="8"/>
-      <c r="M107" s="11"/>
-      <c r="N107" s="10"/>
-    </row>
-    <row r="108" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="K107" s="8"/>
+      <c r="L107" s="7"/>
+      <c r="M107" s="8"/>
+      <c r="N107" s="11"/>
+      <c r="O107" s="10"/>
+    </row>
+    <row r="108" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A108" s="9"/>
       <c r="B108" s="7"/>
       <c r="C108" s="7"/>
@@ -11513,10 +11935,11 @@
       <c r="H108" s="8"/>
       <c r="I108" s="8"/>
       <c r="J108" s="8"/>
-      <c r="K108" s="7"/>
-      <c r="L108" s="8"/>
-      <c r="M108" s="11"/>
-      <c r="N108" s="10"/>
+      <c r="K108" s="8"/>
+      <c r="L108" s="7"/>
+      <c r="M108" s="8"/>
+      <c r="N108" s="11"/>
+      <c r="O108" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>